<commit_message>
Update Notes and their Frequencies.xlsx
</commit_message>
<xml_diff>
--- a/Notes and their Frequencies.xlsx
+++ b/Notes and their Frequencies.xlsx
@@ -1,17 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fbook\Documents\GitHub\tinytapeout\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEA03DF7-E75B-4EC8-806E-9B1354EE6968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Note</t>
   </si>
@@ -53,20 +78,24 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>10khz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -77,36 +106,47 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -296,20 +336,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -317,103 +362,276 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>261.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>261</v>
+      </c>
+      <c r="C2">
+        <v>38</v>
+      </c>
+      <c r="D2" t="str">
+        <f>DEC2BIN(C2)</f>
+        <v>100110</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(F2/B2,0)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>277.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>277</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D13" si="0">DEC2BIN(C3)</f>
+        <v>100100</v>
+      </c>
+      <c r="F3">
+        <v>10000</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="1">ROUND(F3/B3,0)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>293.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>293</v>
+      </c>
+      <c r="C4">
+        <v>34</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>100010</v>
+      </c>
+      <c r="F4">
+        <v>10000</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>311.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>311</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="F5">
+        <v>10000</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>329.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>329</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>11110</v>
+      </c>
+      <c r="F6">
+        <v>10000</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>349.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>349</v>
+      </c>
+      <c r="C7">
+        <v>29</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>11101</v>
+      </c>
+      <c r="F7">
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
-        <v>369.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>369</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>11011</v>
+      </c>
+      <c r="F8">
+        <v>10000</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>392.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>392</v>
+      </c>
+      <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>11010</v>
+      </c>
+      <c r="F9">
+        <v>10000</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>415.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>415</v>
+      </c>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>11000</v>
+      </c>
+      <c r="F10">
+        <v>10000</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1">
-        <v>440.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>440</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>10111</v>
+      </c>
+      <c r="F11">
+        <v>10000</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>466.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>466</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>10101</v>
+      </c>
+      <c r="F12">
+        <v>10000</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1">
-        <v>493.0</v>
+        <v>493</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>10100</v>
+      </c>
+      <c r="F13">
+        <v>10000</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>